<commit_message>
feat: create api send mail survey period
</commit_message>
<xml_diff>
--- a/public/template/template_graduation_student.xlsx
+++ b/public/template/template_graduation_student.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiendam/Dev/Projects/student.resource.vnua/backend/public/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiendam/Documents/Docs_learning/code/tai_lieu_do_an_tot_nghiep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F993170-3909-A045-84A6-4A9F1C2D9925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DA6271-3A35-9844-B9BF-EB44BB77F3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{8F200349-89FF-E64A-B826-9A354B5EF6EF}"/>
+    <workbookView xWindow="8820" yWindow="880" windowWidth="27180" windowHeight="22500" xr2:uid="{8F200349-89FF-E64A-B826-9A354B5EF6EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>STT</t>
   </si>
@@ -46,86 +46,122 @@
     <t>Ngày sinh</t>
   </si>
   <si>
+    <t>Điểm TB</t>
+  </si>
+  <si>
+    <t>Xếp loại</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>Đại học</t>
+  </si>
+  <si>
+    <t>Giỏi</t>
+  </si>
+  <si>
+    <t>Trung bình</t>
+  </si>
+  <si>
+    <t>Lớp</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Hệ đào tạo</t>
+  </si>
+  <si>
+    <t>leha@gmail.com</t>
+  </si>
+  <si>
+    <t>truongan@gmail.com</t>
+  </si>
+  <si>
+    <t>Mã ngành đào tạo</t>
+  </si>
+  <si>
+    <t>CCCD/CMND</t>
+  </si>
+  <si>
+    <t>SĐT</t>
+  </si>
+  <si>
+    <t>0968511442</t>
+  </si>
+  <si>
+    <t>0968511443</t>
+  </si>
+  <si>
+    <t>0968511444</t>
+  </si>
+  <si>
+    <t>an@gmail.com</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>Khá</t>
+  </si>
+  <si>
+    <t>1273187263</t>
+  </si>
+  <si>
+    <t>1273187264</t>
+  </si>
+  <si>
+    <t>1273187265</t>
+  </si>
+  <si>
+    <t>Ngành đào tạo</t>
+  </si>
+  <si>
     <t>Giới tính</t>
   </si>
   <si>
+    <t>Nam</t>
+  </si>
+  <si>
     <t>Nơi sinh</t>
   </si>
   <si>
-    <t>Điểm TB</t>
-  </si>
-  <si>
-    <t>Xếp loại</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Lê Thị Nhật</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>H. Văn Giang-Hưng Yên</t>
-  </si>
-  <si>
-    <t>K61QLKT</t>
-  </si>
-  <si>
-    <t>Đại học</t>
-  </si>
-  <si>
-    <t>Kinh tế</t>
-  </si>
-  <si>
-    <t>Khá</t>
-  </si>
-  <si>
-    <t>lehong@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Lan</t>
-  </si>
-  <si>
-    <t>Văn Lâm - Hưng Yên</t>
-  </si>
-  <si>
-    <t>K62KEB</t>
-  </si>
-  <si>
-    <t>Kế toán</t>
-  </si>
-  <si>
-    <t>Giỏi</t>
-  </si>
-  <si>
-    <t>Trần Thị Hoài</t>
-  </si>
-  <si>
-    <t>Kiến Xương - Thái Bình</t>
-  </si>
-  <si>
-    <t>Trung bình</t>
-  </si>
-  <si>
-    <t>Lớp</t>
-  </si>
-  <si>
-    <t>Họ và tên</t>
-  </si>
-  <si>
-    <t>Ngành đào tạo</t>
-  </si>
-  <si>
-    <t>Hệ đào tạo</t>
+    <t>Nguyễn Thị A</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị B</t>
+  </si>
+  <si>
+    <t>Trần Thị C</t>
+  </si>
+  <si>
+    <t>K62CNPMP</t>
+  </si>
+  <si>
+    <t>01097008631</t>
+  </si>
+  <si>
+    <t>01097008632</t>
+  </si>
+  <si>
+    <t>01097008633</t>
+  </si>
+  <si>
+    <t>Công nghệ phần mềm</t>
+  </si>
+  <si>
+    <t>Hương mạc, Từ sơn, Bắc ninh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +181,12 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,6 +220,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -495,19 +541,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D220C2-8715-4E44-9410-B849AA101EEC}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,155 +574,193 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>637943</v>
+        <v>628012</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D2" s="4">
-        <v>36809</v>
+        <v>36810</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1">
-        <v>3.13</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>637942</v>
+        <v>628013</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4">
         <v>36810</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1">
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="1">
         <v>3.32</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>15</v>
+      <c r="N3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>637942</v>
+        <v>628014</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4">
         <v>36811</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2.29</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>15</v>
+      <c r="O4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
+    <row r="31" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L4" r:id="rId1" xr:uid="{FE97BD5A-EC12-8A44-8368-56BBB1056BE4}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{675EC052-8699-BC44-AB3D-A6F31CA100AF}"/>
-    <hyperlink ref="L2" r:id="rId3" xr:uid="{B2B0795E-F2CB-0E42-A4FE-5D87CB2E8DF6}"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{675EC052-8699-BC44-AB3D-A6F31CA100AF}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{FE97BD5A-EC12-8A44-8368-56BBB1056BE4}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{1D9F9BAA-3E82-734D-A2FE-841C15140204}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>